<commit_message>
updated docs and default task parameters
</commit_message>
<xml_diff>
--- a/stimuli, instructions and parameters.xlsx
+++ b/stimuli, instructions and parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="3" r:id="rId1"/>
@@ -2036,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2149,25 +2149,25 @@
         <v>17</v>
       </c>
       <c r="J2" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K2" s="3">
         <v>1</v>
       </c>
       <c r="L2" s="6">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="M2" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N2" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="O2" s="3">
         <v>1</v>
       </c>
       <c r="P2" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>34</v>

</xml_diff>